<commit_message>
Update Turbine Experimental Data.xlsx
</commit_message>
<xml_diff>
--- a/Turbine Experimental Data.xlsx
+++ b/Turbine Experimental Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thequ\Documents\GitHub\BEP\BEP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Documents\TUD-3\BEP\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B2BE3A3-FD24-4558-A0CF-31A067D237E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FE3CB2-1C63-4C32-A10F-50577E46F104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F95DA856-8800-4DBC-A4BE-C8B7731327AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F95DA856-8800-4DBC-A4BE-C8B7731327AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Load (Ohms)</t>
   </si>
@@ -51,22 +51,133 @@
     <t>Angular velocity (rpm)</t>
   </si>
   <si>
-    <t># coils</t>
-  </si>
-  <si>
     <t>Power (mW)</t>
   </si>
   <si>
-    <t>v=ir</t>
+    <t>k_t</t>
   </si>
   <si>
-    <t>i=v/r</t>
+    <t>T_max</t>
   </si>
   <si>
-    <t>est. Voltage</t>
+    <t>mNm</t>
   </si>
   <si>
-    <t>k_t</t>
+    <t>Coils</t>
+  </si>
+  <si>
+    <t>i_max</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>i_min</t>
+  </si>
+  <si>
+    <t>omega_max</t>
+  </si>
+  <si>
+    <t>rpm</t>
+  </si>
+  <si>
+    <t>Motor constants (datasheet)</t>
+  </si>
+  <si>
+    <t>Motor Constants (calculated)</t>
+  </si>
+  <si>
+    <t>R_motor</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>Nominal Voltage</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>mNm/A</t>
+  </si>
+  <si>
+    <t>k_v</t>
+  </si>
+  <si>
+    <t>mV/(rad/s)</t>
+  </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>Gemiddelde:</t>
+  </si>
+  <si>
+    <t>Standaard deviatie:</t>
+  </si>
+  <si>
+    <t>Air/prop Constants</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>k_t (mNm/A)</t>
+  </si>
+  <si>
+    <t>c_t * u^2 (m^2/s^2)</t>
+  </si>
+  <si>
+    <t>Torque EMK (mNm)</t>
+  </si>
+  <si>
+    <t>T_friction</t>
+  </si>
+  <si>
+    <t>v_in</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>c_t</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>T-test</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>T_0</t>
+  </si>
+  <si>
+    <t>mNm/rpm</t>
+  </si>
+  <si>
+    <t>T_fric = a * rpm + b</t>
+  </si>
+  <si>
+    <t>Torque Friction (mNm)</t>
+  </si>
+  <si>
+    <t>Torque Total (mNm)</t>
   </si>
 </sst>
 </file>
@@ -74,10 +185,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -113,15 +232,21 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +264,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -322,7 +447,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$23</c:f>
+              <c:f>Sheet1!$L$4:$L$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -684,7 +809,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -759,11 +884,188 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$2</c:f>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power (mW)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1070</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0920000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1489999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11253000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22110000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.50634000000000012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6136000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1715</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.6499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.76</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F70A-49CF-99FA-64C2B6C92F5B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -810,7 +1112,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$19</c:f>
+              <c:f>Sheet1!$K$3:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -870,7 +1172,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$19</c:f>
+              <c:f>Sheet1!$L$3:$L$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -931,7 +1233,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C117-49A1-A332-7BF7E09DC79D}"/>
+              <c16:uniqueId val="{00000001-F70A-49CF-99FA-64C2B6C92F5B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1224,6 +1526,1099 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Torque</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NL"/>
+              <a:t> vs. Angular</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NL" baseline="0"/>
+              <a:t> velocity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1410</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1070</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.4418862643278552E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1626332458814942E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.592223097243545E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.518444619448709E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3474801837846536E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9020209974941307E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5414513561070226E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0245928259316117E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1059094488723592E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.6013473316627543E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.9020209974941307E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2026946633255086E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13804041994988261</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13804041994988261</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.11503368329156885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.11503368329156885</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F973-4862-9B45-1C81FBE78644}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="533555568"/>
+        <c:axId val="533553600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="533555568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NL"/>
+                  <a:t>Angular velocity (rpm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533553600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="533553600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Torque</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> (mNm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533555568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL" baseline="0"/>
+              <a:t>c_t vs lambda</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$4:$S$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.7283179278308909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2938046054770549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8592912831232162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4823001646924414</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4194683116206441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5451320177642369</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9168134870462783</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9168134870462783</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8539816339744828</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0371675440411376</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7230082786821574</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5973445725385655</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7805304826052186</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.5238934211693023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0106192982974678</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0053096491487339</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$4:$R$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.38791031847172214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39096258004248241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39418288944481067</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39251775362708674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39297173331644825</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39516277365517011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39550137475958608</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39757725973777885</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40189139696992265</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.40400217155478046</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41222788285568907</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42144926731374616</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.43690501675841475</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.43026719571075783</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.40710638705262109</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.40179613021449556</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5172-4502-9D01-AD9D637545D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="533555568"/>
+        <c:axId val="533553600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="533555568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Lambda</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533553600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="533553600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t>C_t</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533555568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1304,6 +2699,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -2380,20 +3855,1096 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
+      <xdr:colOff>110490</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2423,13 +4974,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>310515</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
@@ -2458,11 +5009,87 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>340995</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423CB697-A7EF-452B-9372-A6CA9184D09F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60BA9F54-6CDC-4E6C-AD87-3DFFA82E1AA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2758,30 +5385,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6E4431-2A3A-4509-91B4-41CDE98B96BE}">
-  <dimension ref="D2:N34"/>
+  <dimension ref="B1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="N1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>11.67</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -2795,23 +5442,43 @@
       <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>0.54</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1">
-        <f>H3/(22.2+F3)</f>
-        <v>3.1499999999300702E-12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2">
         <v>1000000000000</v>
@@ -2825,26 +5492,52 @@
       <c r="I3" s="2">
         <v>126</v>
       </c>
-      <c r="J3" s="2">
-        <f>I3*60/$D$4</f>
+      <c r="K3" s="2">
+        <f>I3*60/$C$5</f>
         <v>1260</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <f>G3*H3*1000</f>
         <v>0</v>
       </c>
-      <c r="L3" s="1">
-        <f>H3/J3 * 1000</f>
-        <v>2.5</v>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:M18" si="0">(H3 + C$10*G3)  /(K3 * PI() / 30) * 1000</f>
+        <v>23.8732414637843</v>
+      </c>
+      <c r="N3" s="1">
+        <f>G3 *M$25</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <f>C$25*K3+C$23</f>
+        <v>0.90507538605439031</v>
+      </c>
+      <c r="P3" s="1">
+        <f>N3+O3</f>
+        <v>0.90507538605439031</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>P3 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.38887831316249483</v>
+      </c>
+      <c r="R3" s="1">
+        <f>Q3/C$18</f>
+        <v>0.38887831316249483</v>
+      </c>
+      <c r="S3" s="1">
+        <f>C$16 / 2 *K3/30*PI() / C$18</f>
+        <v>7.9168134870462783</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D4" s="1">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" ref="E4:E23" si="0">H4/(22.2+F4)</f>
-        <v>2.8818667955296563E-6</v>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="2">
         <v>1002800</v>
@@ -2858,23 +5551,49 @@
       <c r="I4" s="2">
         <v>123</v>
       </c>
-      <c r="J4" s="2">
-        <f t="shared" ref="J4:J23" si="1">I4*60/$D$4</f>
+      <c r="K4" s="2">
+        <f>I4*60/$C$5</f>
         <v>1230</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <f>G4*H4*1000</f>
         <v>8.0920000000000002E-3</v>
       </c>
-      <c r="L4" s="1">
-        <f t="shared" ref="L4:L23" si="2">H4/J4 * 1000</f>
-        <v>2.3495934959349594</v>
+      <c r="M4" s="1">
+        <f t="shared" si="0"/>
+        <v>22.437448219990948</v>
+      </c>
+      <c r="N4" s="1">
+        <f>G4 *M$25</f>
+        <v>6.4418862643278552E-5</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O20" si="1">C$25*K4+C$23</f>
+        <v>0.90275805634844275</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P23" si="2">N4+O4</f>
+        <v>0.90282247521108605</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>P4 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.38791031847172214</v>
+      </c>
+      <c r="R4" s="1">
+        <f>Q4/C$18</f>
+        <v>0.38791031847172214</v>
+      </c>
+      <c r="S4" s="1">
+        <f>C$16 / 2 *K4/30*PI() / C$18</f>
+        <v>7.7283179278308909</v>
       </c>
     </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>1.0065434337012375E-5</v>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
       </c>
       <c r="F5" s="2">
         <v>332800</v>
@@ -2888,23 +5607,52 @@
       <c r="I5" s="2">
         <v>132</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
+        <f>I5*60/$C$5</f>
+        <v>1320</v>
+      </c>
+      <c r="L5" s="1">
+        <f>G5*H5*1000</f>
+        <v>3.1489999999999997E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="0"/>
+        <v>24.236468411685141</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" ref="N4:N23" si="3">G5 *M$25</f>
+        <v>2.1626332458814942E-4</v>
+      </c>
+      <c r="O5" s="1">
         <f t="shared" si="1"/>
-        <v>1320</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" ref="K4:K23" si="3">G5*H5*1000</f>
-        <v>3.1489999999999997E-2</v>
-      </c>
-      <c r="L5" s="1">
+        <v>0.90971004546628531</v>
+      </c>
+      <c r="P5" s="1">
         <f t="shared" si="2"/>
-        <v>2.5378787878787876</v>
+        <v>0.90992630879087344</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>P5 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39096258004248241</v>
+      </c>
+      <c r="R5" s="1">
+        <f>Q5/C$18</f>
+        <v>0.39096258004248241</v>
+      </c>
+      <c r="S5" s="1">
+        <f>C$16 / 2 *K5/30*PI() / C$18</f>
+        <v>8.2938046054770549</v>
       </c>
     </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>3.316404434061905E-5</v>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4500</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F6" s="2">
         <v>102800</v>
@@ -2918,23 +5666,52 @@
       <c r="I6" s="2">
         <v>141</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
+        <f>I6*60/$C$5</f>
+        <v>1410</v>
+      </c>
+      <c r="L6" s="1">
+        <f>G6*H6*1000</f>
+        <v>0.11253000000000001</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="0"/>
+        <v>23.099364662480731</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="3"/>
+        <v>7.592223097243545E-4</v>
+      </c>
+      <c r="O6" s="1">
         <f t="shared" si="1"/>
-        <v>1410</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="3"/>
-        <v>0.11253000000000001</v>
-      </c>
-      <c r="L6" s="1">
+        <v>0.91666203458412787</v>
+      </c>
+      <c r="P6" s="1">
         <f t="shared" si="2"/>
-        <v>2.4184397163120566</v>
+        <v>0.91742125689385223</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>P6 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39418288944481067</v>
+      </c>
+      <c r="R6" s="1">
+        <f>Q6/C$18</f>
+        <v>0.39418288944481067</v>
+      </c>
+      <c r="S6" s="1">
+        <f>C$16 / 2 *K6/30*PI() / C$18</f>
+        <v>8.8592912831232162</v>
       </c>
     </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E7" s="3">
-        <f t="shared" si="0"/>
-        <v>6.7239102247592444E-5</v>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F7" s="2">
         <v>49800</v>
@@ -2948,27 +5725,44 @@
       <c r="I7" s="2">
         <v>135</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
+        <f>I7*60/$C$5</f>
+        <v>1350</v>
+      </c>
+      <c r="L7" s="1">
+        <f>G7*H7*1000</f>
+        <v>0.22110000000000005</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="0"/>
+        <v>23.706777182565222</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="3"/>
+        <v>1.518444619448709E-3</v>
+      </c>
+      <c r="O7" s="1">
         <f t="shared" si="1"/>
-        <v>1350</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="3"/>
-        <v>0.22110000000000005</v>
-      </c>
-      <c r="L7" s="1">
+        <v>0.91202737517223287</v>
+      </c>
+      <c r="P7" s="1">
         <f t="shared" si="2"/>
-        <v>2.4814814814814818</v>
+        <v>0.91354581979168159</v>
+      </c>
+      <c r="Q7" s="1">
+        <f>P7 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39251775362708674</v>
+      </c>
+      <c r="R7" s="1">
+        <f>Q7/C$18</f>
+        <v>0.39251775362708674</v>
+      </c>
+      <c r="S7" s="1">
+        <f>C$16 / 2 *K7/30*PI() / C$18</f>
+        <v>8.4823001646924414</v>
       </c>
     </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.401970816446568E-4</v>
-      </c>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F8" s="2">
         <v>24800</v>
       </c>
@@ -2981,26 +5775,46 @@
       <c r="I8" s="2">
         <v>134</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
+        <f>I8*60/$C$5</f>
+        <v>1340</v>
+      </c>
+      <c r="L8" s="1">
+        <f>G8*H8*1000</f>
+        <v>0.50634000000000012</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>24.822707594438487</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3474801837846536E-3</v>
+      </c>
+      <c r="O8" s="1">
         <f t="shared" si="1"/>
-        <v>1340</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="3"/>
-        <v>0.50634000000000012</v>
-      </c>
-      <c r="L8" s="1">
+        <v>0.91125493193691698</v>
+      </c>
+      <c r="P8" s="1">
         <f t="shared" si="2"/>
-        <v>2.5970149253731343</v>
+        <v>0.91460241212070159</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>P8 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39297173331644825</v>
+      </c>
+      <c r="R8" s="1">
+        <f>Q8/C$18</f>
+        <v>0.39297173331644825</v>
+      </c>
+      <c r="S8" s="1">
+        <f>C$16 / 2 *K8/30*PI() / C$18</f>
+        <v>8.4194683116206441</v>
       </c>
     </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="0"/>
-        <v>3.2428009818203583E-4</v>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="F9" s="2">
         <v>10000</v>
@@ -3014,23 +5828,53 @@
       <c r="I9" s="2">
         <v>136</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
+        <f>I9*60/$C$5</f>
+        <v>1360</v>
+      </c>
+      <c r="L9" s="1">
+        <f>G9*H9*1000</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>22.866820500114962</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="3"/>
+        <v>6.9020209974941307E-3</v>
+      </c>
+      <c r="O9" s="1">
         <f t="shared" si="1"/>
-        <v>1360</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="3"/>
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="L9" s="1">
+        <v>0.91279981840754865</v>
+      </c>
+      <c r="P9" s="1">
         <f t="shared" si="2"/>
-        <v>2.3897058823529416</v>
+        <v>0.9197018394050428</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>P9 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39516277365517011</v>
+      </c>
+      <c r="R9" s="1">
+        <f>Q9/C$18</f>
+        <v>0.39516277365517011</v>
+      </c>
+      <c r="S9" s="1">
+        <f>C$16 / 2 *K9/30*PI() / C$18</f>
+        <v>8.5451320177642369</v>
       </c>
     </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E10" s="3">
-        <f t="shared" si="0"/>
-        <v>6.3529710728050485E-4</v>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <f>C7/C3</f>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F10" s="2">
         <v>4700</v>
@@ -3044,23 +5888,53 @@
       <c r="I10" s="2">
         <v>126</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
+        <f>I10*60/$C$5</f>
+        <v>1260</v>
+      </c>
+      <c r="L10" s="1">
+        <f>G10*H10*1000</f>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>22.849260454261838</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5414513561070226E-2</v>
+      </c>
+      <c r="O10" s="1">
         <f t="shared" si="1"/>
-        <v>1260</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="3"/>
-        <v>2.0100000000000002</v>
-      </c>
-      <c r="L10" s="1">
+        <v>0.90507538605439031</v>
+      </c>
+      <c r="P10" s="1">
         <f t="shared" si="2"/>
-        <v>2.3809523809523814</v>
+        <v>0.92048989961546057</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>P10 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39550137475958608</v>
+      </c>
+      <c r="R10" s="1">
+        <f>Q10/C$18</f>
+        <v>0.39550137475958608</v>
+      </c>
+      <c r="S10" s="1">
+        <f>C$16 / 2 *K10/30*PI() / C$18</f>
+        <v>7.9168134870462783</v>
       </c>
     </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="3">
-        <f t="shared" si="0"/>
-        <v>8.9398591294925062E-4</v>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <f>C2/(C3-C4)</f>
+        <v>23.816326530612244</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="F11" s="2">
         <v>3300</v>
@@ -3074,23 +5948,53 @@
       <c r="I11" s="2">
         <v>126</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
+        <f>I11*60/$C$5</f>
+        <v>1260</v>
+      </c>
+      <c r="L11" s="1">
+        <f>G11*H11*1000</f>
+        <v>2.6136000000000004</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>22.657264014976384</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="3"/>
+        <v>2.0245928259316117E-2</v>
+      </c>
+      <c r="O11" s="1">
         <f t="shared" si="1"/>
-        <v>1260</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="3"/>
-        <v>2.6136000000000004</v>
-      </c>
-      <c r="L11" s="1">
+        <v>0.90507538605439031</v>
+      </c>
+      <c r="P11" s="1">
         <f t="shared" si="2"/>
-        <v>2.3571428571428572</v>
+        <v>0.92532131431370646</v>
+      </c>
+      <c r="Q11" s="1">
+        <f>P11 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.39757725973777885</v>
+      </c>
+      <c r="R11" s="1">
+        <f>Q11/C$18</f>
+        <v>0.39757725973777885</v>
+      </c>
+      <c r="S11" s="1">
+        <f>C$16 / 2 *K11/30*PI() / C$18</f>
+        <v>7.9168134870462783</v>
       </c>
     </row>
-    <row r="12" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>1.3905139051390515E-3</v>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1">
+        <f>(C7-C10*C4)/(C6 * PI() / 30) * 1000</f>
+        <v>23.106939885934434</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="F12" s="2">
         <v>2200</v>
@@ -3104,23 +6008,53 @@
       <c r="I12" s="2">
         <v>125</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
+        <f>I12*60/$C$5</f>
+        <v>1250</v>
+      </c>
+      <c r="L12" s="1">
+        <f>G12*H12*1000</f>
+        <v>4.1715</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>23.835044277442243</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="3"/>
+        <v>3.1059094488723592E-2</v>
+      </c>
+      <c r="O12" s="1">
         <f t="shared" si="1"/>
-        <v>1250</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="3"/>
-        <v>4.1715</v>
-      </c>
-      <c r="L12" s="1">
+        <v>0.90430294281907442</v>
+      </c>
+      <c r="P12" s="1">
         <f t="shared" si="2"/>
-        <v>2.472</v>
+        <v>0.93536203730779799</v>
+      </c>
+      <c r="Q12" s="1">
+        <f>P12 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.40189139696992265</v>
+      </c>
+      <c r="R12" s="1">
+        <f>Q12/C$18</f>
+        <v>0.40189139696992265</v>
+      </c>
+      <c r="S12" s="1">
+        <f>C$16 / 2 *K12/30*PI() / C$18</f>
+        <v>7.8539816339744828</v>
       </c>
     </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6413617687341029E-3</v>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1">
+        <f>C11*C4</f>
+        <v>1.1908163265306122</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F13" s="2">
         <v>1000</v>
@@ -3134,24 +6068,44 @@
       <c r="I13" s="2">
         <v>112</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
+        <f>I13*60/$C$5</f>
+        <v>1120</v>
+      </c>
+      <c r="L13" s="1">
+        <f>G13*H13*1000</f>
+        <v>5.4</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>23.399566037915566</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6013473316627543E-2</v>
+      </c>
+      <c r="O13" s="1">
         <f t="shared" si="1"/>
-        <v>1120</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="3"/>
-        <v>5.4</v>
-      </c>
-      <c r="L13" s="1">
+        <v>0.89426118075996852</v>
+      </c>
+      <c r="P13" s="1">
         <f t="shared" si="2"/>
-        <v>2.410714285714286</v>
+        <v>0.94027465407659605</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>P13 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.40400217155478046</v>
+      </c>
+      <c r="R13" s="1">
+        <f>Q13/C$18</f>
+        <v>0.40400217155478046</v>
+      </c>
+      <c r="S13" s="1">
+        <f>C$16 / 2 *K13/30*PI() / C$18</f>
+        <v>7.0371675440411376</v>
       </c>
     </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E14" s="3">
-        <f t="shared" si="0"/>
-        <v>3.6314440330390196E-3</v>
-      </c>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F14" s="2">
         <v>680</v>
       </c>
@@ -3164,27 +6118,46 @@
       <c r="I14" s="2">
         <v>107</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
+        <f>I14*60/$C$5</f>
+        <v>1070</v>
+      </c>
+      <c r="L14" s="1">
+        <f>G14*H14*1000</f>
+        <v>7.6499999999999995</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>23.352641182642586</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="3"/>
+        <v>6.9020209974941307E-2</v>
+      </c>
+      <c r="O14" s="1">
         <f t="shared" si="1"/>
-        <v>1070</v>
-      </c>
-      <c r="K14" s="1">
-        <f t="shared" si="3"/>
-        <v>7.6499999999999995</v>
-      </c>
-      <c r="L14" s="1">
+        <v>0.89039896458338941</v>
+      </c>
+      <c r="P14" s="1">
         <f t="shared" si="2"/>
-        <v>2.3831775700934581</v>
-      </c>
-      <c r="N14" s="1">
-        <f>AVERAGE(L3:L23)</f>
-        <v>2.3140309809730626</v>
+        <v>0.9594191745583307</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>P14 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.41222788285568907</v>
+      </c>
+      <c r="R14" s="1">
+        <f>Q14/C$18</f>
+        <v>0.41222788285568907</v>
+      </c>
+      <c r="S14" s="1">
+        <f>C$16 / 2 *K14/30*PI() / C$18</f>
+        <v>6.7230082786821574</v>
       </c>
     </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E15" s="3">
-        <f t="shared" si="0"/>
-        <v>4.7541649735879724E-3</v>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="F15" s="2">
         <v>470</v>
@@ -3198,27 +6171,52 @@
       <c r="I15" s="2">
         <v>105</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
+        <f>I15*60/$C$5</f>
+        <v>1050</v>
+      </c>
+      <c r="L15" s="1">
+        <f>G15*H15*1000</f>
+        <v>9.36</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>22.089695593579886</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="3"/>
+        <v>9.2026946633255086E-2</v>
+      </c>
+      <c r="O15" s="1">
         <f t="shared" si="1"/>
-        <v>1050</v>
-      </c>
-      <c r="K15" s="1">
-        <f t="shared" si="3"/>
-        <v>9.36</v>
-      </c>
-      <c r="L15" s="1">
+        <v>0.88885407811275763</v>
+      </c>
+      <c r="P15" s="1">
         <f t="shared" si="2"/>
-        <v>2.2285714285714282</v>
-      </c>
-      <c r="N15" s="1">
-        <f>_xlfn.STDEV.P(L3:L23)</f>
-        <v>0.25996418945232125</v>
+        <v>0.98088102474601269</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>P15 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.42144926731374616</v>
+      </c>
+      <c r="R15" s="1">
+        <f>Q15/C$18</f>
+        <v>0.42144926731374616</v>
+      </c>
+      <c r="S15" s="1">
+        <f>C$16 / 2 *K15/30*PI() / C$18</f>
+        <v>6.5973445725385655</v>
       </c>
     </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E16" s="3">
-        <f t="shared" si="0"/>
-        <v>6.1328790459965936E-3</v>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F16" s="2">
         <v>330</v>
@@ -3232,23 +6230,52 @@
       <c r="I16" s="2">
         <v>92</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
+        <f>I16*60/$C$5</f>
+        <v>920</v>
+      </c>
+      <c r="L16" s="1">
+        <f>G16*H16*1000</f>
+        <v>12.96</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>23.804043662439998</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="3"/>
+        <v>0.13804041994988261</v>
+      </c>
+      <c r="O16" s="1">
         <f t="shared" si="1"/>
-        <v>920</v>
-      </c>
-      <c r="K16" s="1">
-        <f t="shared" si="3"/>
-        <v>12.96</v>
-      </c>
-      <c r="L16" s="1">
+        <v>0.87881231605365184</v>
+      </c>
+      <c r="P16" s="1">
         <f t="shared" si="2"/>
-        <v>2.347826086956522</v>
+        <v>1.0168527360035344</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>P16 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.43690501675841475</v>
+      </c>
+      <c r="R16" s="1">
+        <f>Q16/C$18</f>
+        <v>0.43690501675841475</v>
+      </c>
+      <c r="S16" s="1">
+        <f>C$16 / 2 *K16/30*PI() / C$18</f>
+        <v>5.7805304826052186</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="3">
-        <f t="shared" si="0"/>
-        <v>6.028075970272502E-3</v>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F17" s="2">
         <v>220</v>
@@ -3262,23 +6289,52 @@
       <c r="I17" s="2">
         <v>72</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
+        <f>I17*60/$C$5</f>
+        <v>720</v>
+      </c>
+      <c r="L17" s="1">
+        <f>G17*H17*1000</f>
+        <v>8.76</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>21.132239666090548</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="3"/>
+        <v>0.13804041994988261</v>
+      </c>
+      <c r="O17" s="1">
         <f t="shared" si="1"/>
-        <v>720</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="3"/>
-        <v>8.76</v>
-      </c>
-      <c r="L17" s="1">
+        <v>0.86336345134733505</v>
+      </c>
+      <c r="P17" s="1">
         <f t="shared" si="2"/>
-        <v>2.0277777777777777</v>
+        <v>1.0014038712972178</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>P17 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.43026719571075783</v>
+      </c>
+      <c r="R17" s="1">
+        <f>Q17/C$18</f>
+        <v>0.43026719571075783</v>
+      </c>
+      <c r="S17" s="1">
+        <f>C$16 / 2 *K17/30*PI() / C$18</f>
+        <v>4.5238934211693023</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="3">
-        <f t="shared" si="0"/>
-        <v>5.1554828150572832E-3</v>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F18" s="2">
         <v>100</v>
@@ -3292,24 +6348,44 @@
       <c r="I18" s="2">
         <v>32</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
+        <f>I18*60/$C$5</f>
+        <v>320</v>
+      </c>
+      <c r="L18" s="1">
+        <f>G18*H18*1000</f>
+        <v>3.15</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>22.115905633811291</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11503368329156885</v>
+      </c>
+      <c r="O18" s="1">
         <f t="shared" si="1"/>
-        <v>320</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="3"/>
-        <v>3.15</v>
-      </c>
-      <c r="L18" s="1">
+        <v>0.83246572193470147</v>
+      </c>
+      <c r="P18" s="1">
         <f t="shared" si="2"/>
-        <v>1.96875</v>
+        <v>0.9474994052262703</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>P18 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.40710638705262109</v>
+      </c>
+      <c r="R18" s="1">
+        <f>Q18/C$18</f>
+        <v>0.40710638705262109</v>
+      </c>
+      <c r="S18" s="1">
+        <f>C$16 / 2 *K18/30*PI() / C$18</f>
+        <v>2.0106192982974678</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E19" s="3">
-        <f t="shared" si="0"/>
-        <v>3.4393063583815025E-3</v>
-      </c>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F19" s="2">
         <v>47</v>
       </c>
@@ -3322,24 +6398,44 @@
       <c r="I19" s="2">
         <v>16</v>
       </c>
-      <c r="J19" s="2">
-        <f t="shared" si="1"/>
+      <c r="K19" s="2">
+        <f>I19*60/$C$5</f>
         <v>160</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <f>G19*H19*1000</f>
         <v>1.19</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
+        <f>(H19 + C$10*G19)  /(K19 * PI() / 30) * 1000</f>
+        <v>20.836034633113968</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11503368329156885</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82010663016964813</v>
+      </c>
+      <c r="P19" s="1">
         <f t="shared" si="2"/>
-        <v>1.4874999999999998</v>
+        <v>0.93514031346121695</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>P19 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0.40179613021449556</v>
+      </c>
+      <c r="R19" s="1">
+        <f>Q19/C$18</f>
+        <v>0.40179613021449556</v>
+      </c>
+      <c r="S19" s="1">
+        <f>C$16 / 2 *K19/30*PI() / C$18</f>
+        <v>1.0053096491487339</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F20" s="2">
         <v>10</v>
       </c>
@@ -3352,20 +6448,42 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="J20" s="2">
-        <f t="shared" si="1"/>
+      <c r="K20" s="2">
+        <f>I20*60/$C$5</f>
         <v>0</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <f>G21*H20*1000</f>
         <v>0</v>
       </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" ref="Q20:Q23" si="4">P20 / (0.5*C$17 *C$16^2/4) / 1000</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <f>Q20/C$18</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="1">
+        <f t="shared" ref="S20:S23" si="5">C$16 / 2 *K20/30*PI() / C$18</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F21" s="4">
         <v>4.7</v>
       </c>
@@ -3378,19 +6496,51 @@
       <c r="I21" s="1">
         <v>0</v>
       </c>
-      <c r="J21" s="2">
-        <f t="shared" si="1"/>
+      <c r="K21" s="2">
+        <f>I21*60/$C$5</f>
         <v>0</v>
       </c>
-      <c r="K21" s="1" t="e">
-        <f>#REF!*H21*1000</f>
-        <v>#REF!</v>
+      <c r="L21" s="1">
+        <f t="shared" ref="L21:L23" si="6">G22*H21*1000</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <f>Q21/C$18</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="1">
+        <f>C12*C3</f>
+        <v>12.477747538404595</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F22" s="4">
         <v>1.5</v>
@@ -3401,15 +6551,54 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
-      <c r="K22" s="1">
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <f>I22*60/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <f>Q22/C$18</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="1">
+        <f>C22-C2</f>
+        <v>0.80774753840459468</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -3423,46 +6612,109 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="J23" s="2">
-        <f t="shared" si="1"/>
+      <c r="K23" s="2">
+        <f>I23*60/$C$5</f>
         <v>0</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <f>Q23/C$18</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="1">
+        <f>C12*C4</f>
+        <v>1.1553469942967218</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1">
+        <f>(C24-C23)/C6</f>
+        <v>7.7244323531583815E-5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F25" s="4"/>
+      <c r="J25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="1">
+        <f>AVERAGE(M3:M19)</f>
+        <v>23.00673665831377</v>
+      </c>
     </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F26" s="4"/>
+      <c r="J26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="1">
+        <f>_xlfn.STDEV.S(M3:M19)</f>
+        <v>1.0608381398751274</v>
+      </c>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F34" s="4"/>
     </row>
   </sheetData>
@@ -3475,11 +6727,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A966733-C040-4D9C-93DE-CFC2ED8EA00D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>